<commit_message>
fix error in datafile.
</commit_message>
<xml_diff>
--- a/utilityscripts/as1170_2.xlsx
+++ b/utilityscripts/as1170_2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sean Kane\PycharmProjects\utilityscripts\utilityscripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A89E5E23-32D6-48FE-B97C-D9E451289687}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F04BD463-4757-401C-B0A8-245C895CC616}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -741,7 +741,7 @@
   <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+      <selection activeCell="G26" sqref="G2:G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -791,7 +791,7 @@
       <c r="F2">
         <v>30</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="2">
         <v>1</v>
       </c>
       <c r="H2">
@@ -817,7 +817,7 @@
       <c r="F3">
         <v>30</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="2">
         <v>1</v>
       </c>
       <c r="H3">
@@ -843,7 +843,7 @@
       <c r="F4">
         <v>30</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="2">
         <v>1</v>
       </c>
       <c r="H4">
@@ -869,7 +869,7 @@
       <c r="F5">
         <v>30</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="2">
         <v>1</v>
       </c>
       <c r="H5">
@@ -895,7 +895,7 @@
       <c r="F6">
         <v>30</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="2">
         <v>1</v>
       </c>
       <c r="H6">
@@ -921,7 +921,7 @@
       <c r="F7">
         <v>30</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="2">
         <v>1</v>
       </c>
       <c r="H7">
@@ -947,7 +947,7 @@
       <c r="F8">
         <v>30</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="2">
         <v>1</v>
       </c>
       <c r="H8">
@@ -973,7 +973,7 @@
       <c r="F9">
         <v>34</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="2">
         <v>1</v>
       </c>
       <c r="H9">
@@ -999,7 +999,7 @@
       <c r="F10">
         <v>26</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="2">
         <v>1</v>
       </c>
       <c r="H10">
@@ -1025,7 +1025,7 @@
       <c r="F11">
         <v>23</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="2">
         <v>1.05</v>
       </c>
       <c r="H11">
@@ -1051,8 +1051,8 @@
       <c r="F12">
         <v>23</v>
       </c>
-      <c r="G12">
-        <v>1.05</v>
+      <c r="G12" s="2">
+        <v>1.1000000000000001</v>
       </c>
       <c r="H12">
         <v>50</v>
@@ -1077,7 +1077,7 @@
       <c r="F13">
         <v>30</v>
       </c>
-      <c r="G13">
+      <c r="G13" s="2">
         <v>1</v>
       </c>
       <c r="H13">
@@ -1103,7 +1103,7 @@
       <c r="F14">
         <v>30</v>
       </c>
-      <c r="G14">
+      <c r="G14" s="2">
         <v>1</v>
       </c>
       <c r="H14">
@@ -1129,7 +1129,7 @@
       <c r="F15">
         <v>30</v>
       </c>
-      <c r="G15">
+      <c r="G15" s="2">
         <v>1</v>
       </c>
       <c r="H15">
@@ -1155,7 +1155,7 @@
       <c r="F16">
         <v>30</v>
       </c>
-      <c r="G16">
+      <c r="G16" s="2">
         <v>1</v>
       </c>
       <c r="H16">
@@ -1181,7 +1181,7 @@
       <c r="F17">
         <v>30</v>
       </c>
-      <c r="G17">
+      <c r="G17" s="2">
         <v>1</v>
       </c>
       <c r="H17">
@@ -1207,7 +1207,7 @@
       <c r="F18">
         <v>30</v>
       </c>
-      <c r="G18">
+      <c r="G18" s="2">
         <v>1</v>
       </c>
       <c r="H18">
@@ -1233,7 +1233,7 @@
       <c r="F19">
         <v>26</v>
       </c>
-      <c r="G19">
+      <c r="G19" s="2">
         <v>1</v>
       </c>
       <c r="H19">
@@ -1259,7 +1259,7 @@
       <c r="F20">
         <v>26</v>
       </c>
-      <c r="G20">
+      <c r="G20" s="2">
         <v>1.05</v>
       </c>
       <c r="H20">
@@ -1285,7 +1285,7 @@
       <c r="F21">
         <v>23</v>
       </c>
-      <c r="G21">
+      <c r="G21" s="2">
         <v>1.05</v>
       </c>
       <c r="H21">
@@ -1311,7 +1311,7 @@
       <c r="F22">
         <v>23</v>
       </c>
-      <c r="G22">
+      <c r="G22" s="2">
         <v>1.05</v>
       </c>
       <c r="H22">
@@ -1337,7 +1337,7 @@
       <c r="F23">
         <v>31</v>
       </c>
-      <c r="G23">
+      <c r="G23" s="2">
         <v>1</v>
       </c>
       <c r="H23">
@@ -1363,7 +1363,7 @@
       <c r="F24">
         <v>31</v>
       </c>
-      <c r="G24">
+      <c r="G24" s="2">
         <v>1</v>
       </c>
       <c r="H24">
@@ -1389,7 +1389,7 @@
       <c r="F25">
         <v>37</v>
       </c>
-      <c r="G25">
+      <c r="G25" s="2">
         <v>1</v>
       </c>
       <c r="H25">
@@ -1415,7 +1415,7 @@
       <c r="F26">
         <v>38</v>
       </c>
-      <c r="G26">
+      <c r="G26" s="2">
         <v>1</v>
       </c>
       <c r="H26">

</xml_diff>

<commit_message>
updating code to use .xlsx file.
</commit_message>
<xml_diff>
--- a/utilityscripts/as1170_2.xlsx
+++ b/utilityscripts/as1170_2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sean Kane\PycharmProjects\utilityscripts\utilityscripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F04BD463-4757-401C-B0A8-245C895CC616}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C12CC55-2D5A-44E6-AD99-E14A578D659D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="wind_direction_definitions" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="555" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="554" uniqueCount="44">
   <si>
     <t>N</t>
   </si>
@@ -61,12 +61,6 @@
   </si>
   <si>
     <t>NW</t>
-  </si>
-  <si>
-    <t>Angle</t>
-  </si>
-  <si>
-    <t>Direction</t>
   </si>
   <si>
     <t>standard</t>
@@ -135,16 +129,10 @@
     <t>NZ4</t>
   </si>
   <si>
-    <t>Standard</t>
-  </si>
-  <si>
     <t>ANY</t>
   </si>
   <si>
     <t>F_not_clad</t>
-  </si>
-  <si>
-    <t>Region</t>
   </si>
   <si>
     <t>terrain_cat</t>
@@ -175,6 +163,12 @@
   </si>
   <si>
     <t>m_c_min_r</t>
+  </si>
+  <si>
+    <t>angle</t>
+  </si>
+  <si>
+    <t>wind_region</t>
   </si>
 </sst>
 </file>
@@ -525,96 +519,88 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" customWidth="1"/>
+    <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>8</v>
+        <v>35</v>
       </c>
       <c r="B1" t="s">
-        <v>9</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3">
         <v>45</v>
       </c>
-      <c r="B3" t="s">
-        <v>1</v>
-      </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4">
         <v>90</v>
       </c>
-      <c r="B4" t="s">
-        <v>2</v>
-      </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5">
         <v>135</v>
       </c>
-      <c r="B5" t="s">
-        <v>3</v>
-      </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6">
         <v>180</v>
       </c>
-      <c r="B6" t="s">
-        <v>4</v>
-      </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7">
         <v>225</v>
       </c>
-      <c r="B7" t="s">
-        <v>5</v>
-      </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8">
         <v>270</v>
       </c>
-      <c r="B8" t="s">
-        <v>6</v>
-      </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9">
         <v>315</v>
-      </c>
-      <c r="B9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>360</v>
-      </c>
-      <c r="B10" t="s">
-        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -634,13 +620,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B1" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -740,36 +726,36 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B69B880A-B446-47BA-A657-EACA3F1BE1B1}">
   <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G26" sqref="G2:G26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
         <v>10</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" t="s">
         <v>11</v>
       </c>
-      <c r="C1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E1" t="s">
-        <v>13</v>
-      </c>
       <c r="F1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="G1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="H1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -777,7 +763,7 @@
         <v>2011</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C2">
         <v>67</v>
@@ -803,7 +789,7 @@
         <v>2011</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C3">
         <v>67</v>
@@ -829,7 +815,7 @@
         <v>2011</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C4">
         <v>67</v>
@@ -855,7 +841,7 @@
         <v>2011</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C5">
         <v>67</v>
@@ -881,7 +867,7 @@
         <v>2011</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C6">
         <v>67</v>
@@ -907,7 +893,7 @@
         <v>2011</v>
       </c>
       <c r="B7" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C7">
         <v>67</v>
@@ -933,7 +919,7 @@
         <v>2011</v>
       </c>
       <c r="B8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C8">
         <v>67</v>
@@ -985,7 +971,7 @@
         <v>2011</v>
       </c>
       <c r="B10" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C10">
         <v>106</v>
@@ -1011,7 +997,7 @@
         <v>2011</v>
       </c>
       <c r="B11" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C11">
         <v>122</v>
@@ -1037,7 +1023,7 @@
         <v>2011</v>
       </c>
       <c r="B12" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C12">
         <v>156</v>
@@ -1063,7 +1049,7 @@
         <v>2021</v>
       </c>
       <c r="B13" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C13">
         <v>67</v>
@@ -1089,7 +1075,7 @@
         <v>2021</v>
       </c>
       <c r="B14" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C14">
         <v>67</v>
@@ -1115,7 +1101,7 @@
         <v>2021</v>
       </c>
       <c r="B15" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C15">
         <v>67</v>
@@ -1141,7 +1127,7 @@
         <v>2021</v>
       </c>
       <c r="B16" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C16">
         <v>67</v>
@@ -1167,7 +1153,7 @@
         <v>2021</v>
       </c>
       <c r="B17" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C17">
         <v>67</v>
@@ -1193,7 +1179,7 @@
         <v>2021</v>
       </c>
       <c r="B18" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C18">
         <v>67</v>
@@ -1219,7 +1205,7 @@
         <v>2021</v>
       </c>
       <c r="B19" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C19">
         <v>106</v>
@@ -1245,7 +1231,7 @@
         <v>2021</v>
       </c>
       <c r="B20" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C20">
         <v>106</v>
@@ -1271,7 +1257,7 @@
         <v>2021</v>
       </c>
       <c r="B21" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C21">
         <v>122</v>
@@ -1297,7 +1283,7 @@
         <v>2021</v>
       </c>
       <c r="B22" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C22">
         <v>156</v>
@@ -1323,7 +1309,7 @@
         <v>2021</v>
       </c>
       <c r="B23" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C23">
         <v>61</v>
@@ -1349,7 +1335,7 @@
         <v>2021</v>
       </c>
       <c r="B24" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C24">
         <v>61</v>
@@ -1375,7 +1361,7 @@
         <v>2021</v>
       </c>
       <c r="B25" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C25">
         <v>61</v>
@@ -1401,7 +1387,7 @@
         <v>2021</v>
       </c>
       <c r="B26" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C26">
         <v>61</v>
@@ -1431,8 +1417,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3C7BDFC-6B29-40E5-BF2C-CEB96896C4AA}">
   <dimension ref="A1:D251"/>
   <sheetViews>
-    <sheetView topLeftCell="A175" workbookViewId="0">
-      <selection activeCell="D251" sqref="D2:D251"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1445,16 +1431,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>32</v>
+        <v>8</v>
       </c>
       <c r="B1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" t="s">
         <v>35</v>
       </c>
-      <c r="C1" t="s">
-        <v>39</v>
-      </c>
       <c r="D1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -1462,7 +1448,7 @@
         <v>2011</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C2" t="s">
         <v>0</v>
@@ -1476,7 +1462,7 @@
         <v>2011</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C3" t="s">
         <v>1</v>
@@ -1490,7 +1476,7 @@
         <v>2011</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C4" t="s">
         <v>2</v>
@@ -1504,7 +1490,7 @@
         <v>2011</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C5" t="s">
         <v>3</v>
@@ -1518,7 +1504,7 @@
         <v>2011</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -1532,7 +1518,7 @@
         <v>2011</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C7" t="s">
         <v>5</v>
@@ -1546,7 +1532,7 @@
         <v>2011</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C8" t="s">
         <v>6</v>
@@ -1560,7 +1546,7 @@
         <v>2011</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C9" t="s">
         <v>7</v>
@@ -1574,10 +1560,10 @@
         <v>2011</v>
       </c>
       <c r="B10" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C10" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D10" s="2">
         <v>1</v>
@@ -1588,10 +1574,10 @@
         <v>2011</v>
       </c>
       <c r="B11" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C11" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D11" s="2">
         <v>1</v>
@@ -1602,7 +1588,7 @@
         <v>2011</v>
       </c>
       <c r="B12" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C12" t="s">
         <v>0</v>
@@ -1616,7 +1602,7 @@
         <v>2011</v>
       </c>
       <c r="B13" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C13" t="s">
         <v>1</v>
@@ -1630,7 +1616,7 @@
         <v>2011</v>
       </c>
       <c r="B14" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C14" t="s">
         <v>2</v>
@@ -1644,7 +1630,7 @@
         <v>2011</v>
       </c>
       <c r="B15" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C15" t="s">
         <v>3</v>
@@ -1658,7 +1644,7 @@
         <v>2011</v>
       </c>
       <c r="B16" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C16" t="s">
         <v>4</v>
@@ -1672,7 +1658,7 @@
         <v>2011</v>
       </c>
       <c r="B17" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C17" t="s">
         <v>5</v>
@@ -1686,7 +1672,7 @@
         <v>2011</v>
       </c>
       <c r="B18" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C18" t="s">
         <v>6</v>
@@ -1700,7 +1686,7 @@
         <v>2011</v>
       </c>
       <c r="B19" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C19" t="s">
         <v>7</v>
@@ -1714,10 +1700,10 @@
         <v>2011</v>
       </c>
       <c r="B20" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C20" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D20" s="2">
         <v>1</v>
@@ -1728,10 +1714,10 @@
         <v>2011</v>
       </c>
       <c r="B21" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C21" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D21" s="2">
         <v>1</v>
@@ -1742,7 +1728,7 @@
         <v>2011</v>
       </c>
       <c r="B22" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C22" t="s">
         <v>0</v>
@@ -1756,7 +1742,7 @@
         <v>2011</v>
       </c>
       <c r="B23" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C23" t="s">
         <v>1</v>
@@ -1770,7 +1756,7 @@
         <v>2011</v>
       </c>
       <c r="B24" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C24" t="s">
         <v>2</v>
@@ -1784,7 +1770,7 @@
         <v>2011</v>
       </c>
       <c r="B25" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C25" t="s">
         <v>3</v>
@@ -1798,7 +1784,7 @@
         <v>2011</v>
       </c>
       <c r="B26" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C26" t="s">
         <v>4</v>
@@ -1812,7 +1798,7 @@
         <v>2011</v>
       </c>
       <c r="B27" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C27" t="s">
         <v>5</v>
@@ -1826,7 +1812,7 @@
         <v>2011</v>
       </c>
       <c r="B28" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C28" t="s">
         <v>6</v>
@@ -1840,7 +1826,7 @@
         <v>2011</v>
       </c>
       <c r="B29" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C29" t="s">
         <v>7</v>
@@ -1854,10 +1840,10 @@
         <v>2011</v>
       </c>
       <c r="B30" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C30" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D30" s="2">
         <v>1</v>
@@ -1868,10 +1854,10 @@
         <v>2011</v>
       </c>
       <c r="B31" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C31" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D31" s="2">
         <v>1</v>
@@ -1882,7 +1868,7 @@
         <v>2011</v>
       </c>
       <c r="B32" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C32" t="s">
         <v>0</v>
@@ -1896,7 +1882,7 @@
         <v>2011</v>
       </c>
       <c r="B33" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C33" t="s">
         <v>1</v>
@@ -1910,7 +1896,7 @@
         <v>2011</v>
       </c>
       <c r="B34" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C34" t="s">
         <v>2</v>
@@ -1924,7 +1910,7 @@
         <v>2011</v>
       </c>
       <c r="B35" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C35" t="s">
         <v>3</v>
@@ -1938,7 +1924,7 @@
         <v>2011</v>
       </c>
       <c r="B36" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C36" t="s">
         <v>4</v>
@@ -1952,7 +1938,7 @@
         <v>2011</v>
       </c>
       <c r="B37" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C37" t="s">
         <v>5</v>
@@ -1966,7 +1952,7 @@
         <v>2011</v>
       </c>
       <c r="B38" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C38" t="s">
         <v>6</v>
@@ -1980,7 +1966,7 @@
         <v>2011</v>
       </c>
       <c r="B39" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C39" t="s">
         <v>7</v>
@@ -1994,10 +1980,10 @@
         <v>2011</v>
       </c>
       <c r="B40" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C40" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D40" s="2">
         <v>1</v>
@@ -2008,10 +1994,10 @@
         <v>2011</v>
       </c>
       <c r="B41" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C41" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D41" s="2">
         <v>1</v>
@@ -2022,7 +2008,7 @@
         <v>2011</v>
       </c>
       <c r="B42" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C42" t="s">
         <v>0</v>
@@ -2036,7 +2022,7 @@
         <v>2011</v>
       </c>
       <c r="B43" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C43" t="s">
         <v>1</v>
@@ -2050,7 +2036,7 @@
         <v>2011</v>
       </c>
       <c r="B44" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C44" t="s">
         <v>2</v>
@@ -2064,7 +2050,7 @@
         <v>2011</v>
       </c>
       <c r="B45" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C45" t="s">
         <v>3</v>
@@ -2078,7 +2064,7 @@
         <v>2011</v>
       </c>
       <c r="B46" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C46" t="s">
         <v>4</v>
@@ -2092,7 +2078,7 @@
         <v>2011</v>
       </c>
       <c r="B47" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C47" t="s">
         <v>5</v>
@@ -2106,7 +2092,7 @@
         <v>2011</v>
       </c>
       <c r="B48" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C48" t="s">
         <v>6</v>
@@ -2120,7 +2106,7 @@
         <v>2011</v>
       </c>
       <c r="B49" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C49" t="s">
         <v>7</v>
@@ -2134,10 +2120,10 @@
         <v>2011</v>
       </c>
       <c r="B50" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C50" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D50" s="2">
         <v>1</v>
@@ -2148,10 +2134,10 @@
         <v>2011</v>
       </c>
       <c r="B51" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C51" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D51" s="2">
         <v>1</v>
@@ -2162,7 +2148,7 @@
         <v>2011</v>
       </c>
       <c r="B52" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C52" t="s">
         <v>0</v>
@@ -2176,7 +2162,7 @@
         <v>2011</v>
       </c>
       <c r="B53" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C53" t="s">
         <v>1</v>
@@ -2190,7 +2176,7 @@
         <v>2011</v>
       </c>
       <c r="B54" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C54" t="s">
         <v>2</v>
@@ -2204,7 +2190,7 @@
         <v>2011</v>
       </c>
       <c r="B55" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C55" t="s">
         <v>3</v>
@@ -2218,7 +2204,7 @@
         <v>2011</v>
       </c>
       <c r="B56" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C56" t="s">
         <v>4</v>
@@ -2232,7 +2218,7 @@
         <v>2011</v>
       </c>
       <c r="B57" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C57" t="s">
         <v>5</v>
@@ -2246,7 +2232,7 @@
         <v>2011</v>
       </c>
       <c r="B58" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C58" t="s">
         <v>6</v>
@@ -2260,7 +2246,7 @@
         <v>2011</v>
       </c>
       <c r="B59" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C59" t="s">
         <v>7</v>
@@ -2274,10 +2260,10 @@
         <v>2011</v>
       </c>
       <c r="B60" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C60" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D60" s="2">
         <v>1</v>
@@ -2288,10 +2274,10 @@
         <v>2011</v>
       </c>
       <c r="B61" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C61" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D61" s="2">
         <v>1</v>
@@ -2302,7 +2288,7 @@
         <v>2011</v>
       </c>
       <c r="B62" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C62" t="s">
         <v>0</v>
@@ -2316,7 +2302,7 @@
         <v>2011</v>
       </c>
       <c r="B63" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C63" t="s">
         <v>1</v>
@@ -2330,7 +2316,7 @@
         <v>2011</v>
       </c>
       <c r="B64" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C64" t="s">
         <v>2</v>
@@ -2344,7 +2330,7 @@
         <v>2011</v>
       </c>
       <c r="B65" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C65" t="s">
         <v>3</v>
@@ -2358,7 +2344,7 @@
         <v>2011</v>
       </c>
       <c r="B66" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C66" t="s">
         <v>4</v>
@@ -2372,7 +2358,7 @@
         <v>2011</v>
       </c>
       <c r="B67" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C67" t="s">
         <v>5</v>
@@ -2386,7 +2372,7 @@
         <v>2011</v>
       </c>
       <c r="B68" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C68" t="s">
         <v>6</v>
@@ -2400,7 +2386,7 @@
         <v>2011</v>
       </c>
       <c r="B69" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C69" t="s">
         <v>7</v>
@@ -2414,10 +2400,10 @@
         <v>2011</v>
       </c>
       <c r="B70" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C70" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D70" s="2">
         <v>1</v>
@@ -2428,10 +2414,10 @@
         <v>2011</v>
       </c>
       <c r="B71" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C71" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D71" s="2">
         <v>1</v>
@@ -2557,7 +2543,7 @@
         <v>6</v>
       </c>
       <c r="C80" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D80" s="2">
         <v>1</v>
@@ -2571,7 +2557,7 @@
         <v>6</v>
       </c>
       <c r="C81" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D81" s="2">
         <v>1</v>
@@ -2582,7 +2568,7 @@
         <v>2011</v>
       </c>
       <c r="B82" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C82" t="s">
         <v>0</v>
@@ -2596,7 +2582,7 @@
         <v>2011</v>
       </c>
       <c r="B83" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C83" t="s">
         <v>1</v>
@@ -2610,7 +2596,7 @@
         <v>2011</v>
       </c>
       <c r="B84" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C84" t="s">
         <v>2</v>
@@ -2624,7 +2610,7 @@
         <v>2011</v>
       </c>
       <c r="B85" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C85" t="s">
         <v>3</v>
@@ -2638,7 +2624,7 @@
         <v>2011</v>
       </c>
       <c r="B86" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C86" t="s">
         <v>4</v>
@@ -2652,7 +2638,7 @@
         <v>2011</v>
       </c>
       <c r="B87" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C87" t="s">
         <v>5</v>
@@ -2666,7 +2652,7 @@
         <v>2011</v>
       </c>
       <c r="B88" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C88" t="s">
         <v>6</v>
@@ -2680,7 +2666,7 @@
         <v>2011</v>
       </c>
       <c r="B89" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C89" t="s">
         <v>7</v>
@@ -2694,10 +2680,10 @@
         <v>2011</v>
       </c>
       <c r="B90" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C90" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D90" s="2">
         <v>1</v>
@@ -2708,10 +2694,10 @@
         <v>2011</v>
       </c>
       <c r="B91" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C91" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D91" s="2">
         <v>0.95</v>
@@ -2722,7 +2708,7 @@
         <v>2011</v>
       </c>
       <c r="B92" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C92" t="s">
         <v>0</v>
@@ -2736,7 +2722,7 @@
         <v>2011</v>
       </c>
       <c r="B93" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C93" t="s">
         <v>1</v>
@@ -2750,7 +2736,7 @@
         <v>2011</v>
       </c>
       <c r="B94" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C94" t="s">
         <v>2</v>
@@ -2764,7 +2750,7 @@
         <v>2011</v>
       </c>
       <c r="B95" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C95" t="s">
         <v>3</v>
@@ -2778,7 +2764,7 @@
         <v>2011</v>
       </c>
       <c r="B96" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C96" t="s">
         <v>4</v>
@@ -2792,7 +2778,7 @@
         <v>2011</v>
       </c>
       <c r="B97" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C97" t="s">
         <v>5</v>
@@ -2806,7 +2792,7 @@
         <v>2011</v>
       </c>
       <c r="B98" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C98" t="s">
         <v>6</v>
@@ -2820,7 +2806,7 @@
         <v>2011</v>
       </c>
       <c r="B99" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C99" t="s">
         <v>7</v>
@@ -2834,10 +2820,10 @@
         <v>2011</v>
       </c>
       <c r="B100" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C100" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D100" s="2">
         <v>1</v>
@@ -2848,10 +2834,10 @@
         <v>2011</v>
       </c>
       <c r="B101" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C101" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D101" s="2">
         <v>0.95</v>
@@ -2862,7 +2848,7 @@
         <v>2011</v>
       </c>
       <c r="B102" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C102" t="s">
         <v>0</v>
@@ -2876,7 +2862,7 @@
         <v>2011</v>
       </c>
       <c r="B103" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C103" t="s">
         <v>1</v>
@@ -2890,7 +2876,7 @@
         <v>2011</v>
       </c>
       <c r="B104" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C104" t="s">
         <v>2</v>
@@ -2904,7 +2890,7 @@
         <v>2011</v>
       </c>
       <c r="B105" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C105" t="s">
         <v>3</v>
@@ -2918,7 +2904,7 @@
         <v>2011</v>
       </c>
       <c r="B106" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C106" t="s">
         <v>4</v>
@@ -2932,7 +2918,7 @@
         <v>2011</v>
       </c>
       <c r="B107" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C107" t="s">
         <v>5</v>
@@ -2946,7 +2932,7 @@
         <v>2011</v>
       </c>
       <c r="B108" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C108" t="s">
         <v>6</v>
@@ -2960,7 +2946,7 @@
         <v>2011</v>
       </c>
       <c r="B109" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C109" t="s">
         <v>7</v>
@@ -2974,10 +2960,10 @@
         <v>2011</v>
       </c>
       <c r="B110" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C110" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D110" s="2">
         <v>1</v>
@@ -2988,10 +2974,10 @@
         <v>2011</v>
       </c>
       <c r="B111" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C111" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D111" s="2">
         <v>0.95</v>
@@ -3002,7 +2988,7 @@
         <v>2021</v>
       </c>
       <c r="B112" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C112" t="s">
         <v>0</v>
@@ -3016,7 +3002,7 @@
         <v>2021</v>
       </c>
       <c r="B113" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C113" t="s">
         <v>1</v>
@@ -3030,7 +3016,7 @@
         <v>2021</v>
       </c>
       <c r="B114" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C114" t="s">
         <v>2</v>
@@ -3044,7 +3030,7 @@
         <v>2021</v>
       </c>
       <c r="B115" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C115" t="s">
         <v>3</v>
@@ -3058,7 +3044,7 @@
         <v>2021</v>
       </c>
       <c r="B116" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C116" t="s">
         <v>4</v>
@@ -3072,7 +3058,7 @@
         <v>2021</v>
       </c>
       <c r="B117" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C117" t="s">
         <v>5</v>
@@ -3086,7 +3072,7 @@
         <v>2021</v>
       </c>
       <c r="B118" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C118" t="s">
         <v>6</v>
@@ -3100,7 +3086,7 @@
         <v>2021</v>
       </c>
       <c r="B119" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C119" t="s">
         <v>7</v>
@@ -3114,10 +3100,10 @@
         <v>2021</v>
       </c>
       <c r="B120" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C120" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D120" s="2">
         <v>1</v>
@@ -3128,10 +3114,10 @@
         <v>2021</v>
       </c>
       <c r="B121" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C121" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D121" s="2">
         <v>1</v>
@@ -3142,7 +3128,7 @@
         <v>2021</v>
       </c>
       <c r="B122" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C122" t="s">
         <v>0</v>
@@ -3156,7 +3142,7 @@
         <v>2021</v>
       </c>
       <c r="B123" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C123" t="s">
         <v>1</v>
@@ -3170,7 +3156,7 @@
         <v>2021</v>
       </c>
       <c r="B124" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C124" t="s">
         <v>2</v>
@@ -3184,7 +3170,7 @@
         <v>2021</v>
       </c>
       <c r="B125" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C125" t="s">
         <v>3</v>
@@ -3198,7 +3184,7 @@
         <v>2021</v>
       </c>
       <c r="B126" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C126" t="s">
         <v>4</v>
@@ -3212,7 +3198,7 @@
         <v>2021</v>
       </c>
       <c r="B127" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C127" t="s">
         <v>5</v>
@@ -3226,7 +3212,7 @@
         <v>2021</v>
       </c>
       <c r="B128" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C128" t="s">
         <v>6</v>
@@ -3240,7 +3226,7 @@
         <v>2021</v>
       </c>
       <c r="B129" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C129" t="s">
         <v>7</v>
@@ -3254,10 +3240,10 @@
         <v>2021</v>
       </c>
       <c r="B130" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C130" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D130" s="2">
         <v>1</v>
@@ -3268,10 +3254,10 @@
         <v>2021</v>
       </c>
       <c r="B131" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C131" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D131" s="2">
         <v>1</v>
@@ -3282,7 +3268,7 @@
         <v>2021</v>
       </c>
       <c r="B132" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C132" t="s">
         <v>0</v>
@@ -3296,7 +3282,7 @@
         <v>2021</v>
       </c>
       <c r="B133" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C133" t="s">
         <v>1</v>
@@ -3310,7 +3296,7 @@
         <v>2021</v>
       </c>
       <c r="B134" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C134" t="s">
         <v>2</v>
@@ -3324,7 +3310,7 @@
         <v>2021</v>
       </c>
       <c r="B135" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C135" t="s">
         <v>3</v>
@@ -3338,7 +3324,7 @@
         <v>2021</v>
       </c>
       <c r="B136" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C136" t="s">
         <v>4</v>
@@ -3352,7 +3338,7 @@
         <v>2021</v>
       </c>
       <c r="B137" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C137" t="s">
         <v>5</v>
@@ -3366,7 +3352,7 @@
         <v>2021</v>
       </c>
       <c r="B138" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C138" t="s">
         <v>6</v>
@@ -3380,7 +3366,7 @@
         <v>2021</v>
       </c>
       <c r="B139" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C139" t="s">
         <v>7</v>
@@ -3394,10 +3380,10 @@
         <v>2021</v>
       </c>
       <c r="B140" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C140" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D140" s="2">
         <v>1</v>
@@ -3408,10 +3394,10 @@
         <v>2021</v>
       </c>
       <c r="B141" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C141" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D141" s="2">
         <v>1</v>
@@ -3422,7 +3408,7 @@
         <v>2021</v>
       </c>
       <c r="B142" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C142" t="s">
         <v>0</v>
@@ -3436,7 +3422,7 @@
         <v>2021</v>
       </c>
       <c r="B143" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C143" t="s">
         <v>1</v>
@@ -3450,7 +3436,7 @@
         <v>2021</v>
       </c>
       <c r="B144" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C144" t="s">
         <v>2</v>
@@ -3464,7 +3450,7 @@
         <v>2021</v>
       </c>
       <c r="B145" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C145" t="s">
         <v>3</v>
@@ -3478,7 +3464,7 @@
         <v>2021</v>
       </c>
       <c r="B146" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C146" t="s">
         <v>4</v>
@@ -3492,7 +3478,7 @@
         <v>2021</v>
       </c>
       <c r="B147" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C147" t="s">
         <v>5</v>
@@ -3506,7 +3492,7 @@
         <v>2021</v>
       </c>
       <c r="B148" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C148" t="s">
         <v>6</v>
@@ -3520,7 +3506,7 @@
         <v>2021</v>
       </c>
       <c r="B149" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C149" t="s">
         <v>7</v>
@@ -3534,10 +3520,10 @@
         <v>2021</v>
       </c>
       <c r="B150" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C150" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D150" s="2">
         <v>1</v>
@@ -3548,10 +3534,10 @@
         <v>2021</v>
       </c>
       <c r="B151" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C151" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D151" s="2">
         <v>1</v>
@@ -3562,7 +3548,7 @@
         <v>2021</v>
       </c>
       <c r="B152" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C152" t="s">
         <v>0</v>
@@ -3576,7 +3562,7 @@
         <v>2021</v>
       </c>
       <c r="B153" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C153" t="s">
         <v>1</v>
@@ -3590,7 +3576,7 @@
         <v>2021</v>
       </c>
       <c r="B154" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C154" t="s">
         <v>2</v>
@@ -3604,7 +3590,7 @@
         <v>2021</v>
       </c>
       <c r="B155" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C155" t="s">
         <v>3</v>
@@ -3618,7 +3604,7 @@
         <v>2021</v>
       </c>
       <c r="B156" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C156" t="s">
         <v>4</v>
@@ -3632,7 +3618,7 @@
         <v>2021</v>
       </c>
       <c r="B157" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C157" t="s">
         <v>5</v>
@@ -3646,7 +3632,7 @@
         <v>2021</v>
       </c>
       <c r="B158" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C158" t="s">
         <v>6</v>
@@ -3660,7 +3646,7 @@
         <v>2021</v>
       </c>
       <c r="B159" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C159" t="s">
         <v>7</v>
@@ -3674,10 +3660,10 @@
         <v>2021</v>
       </c>
       <c r="B160" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C160" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D160" s="2">
         <v>1</v>
@@ -3688,10 +3674,10 @@
         <v>2021</v>
       </c>
       <c r="B161" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C161" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D161" s="2">
         <v>1</v>
@@ -3702,7 +3688,7 @@
         <v>2021</v>
       </c>
       <c r="B162" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C162" t="s">
         <v>0</v>
@@ -3716,7 +3702,7 @@
         <v>2021</v>
       </c>
       <c r="B163" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C163" t="s">
         <v>1</v>
@@ -3730,7 +3716,7 @@
         <v>2021</v>
       </c>
       <c r="B164" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C164" t="s">
         <v>2</v>
@@ -3744,7 +3730,7 @@
         <v>2021</v>
       </c>
       <c r="B165" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C165" t="s">
         <v>3</v>
@@ -3758,7 +3744,7 @@
         <v>2021</v>
       </c>
       <c r="B166" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C166" t="s">
         <v>4</v>
@@ -3772,7 +3758,7 @@
         <v>2021</v>
       </c>
       <c r="B167" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C167" t="s">
         <v>5</v>
@@ -3786,7 +3772,7 @@
         <v>2021</v>
       </c>
       <c r="B168" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C168" t="s">
         <v>6</v>
@@ -3800,7 +3786,7 @@
         <v>2021</v>
       </c>
       <c r="B169" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C169" t="s">
         <v>7</v>
@@ -3814,10 +3800,10 @@
         <v>2021</v>
       </c>
       <c r="B170" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C170" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D170" s="2">
         <v>1</v>
@@ -3828,10 +3814,10 @@
         <v>2021</v>
       </c>
       <c r="B171" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C171" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D171" s="2">
         <v>1</v>
@@ -3842,7 +3828,7 @@
         <v>2021</v>
       </c>
       <c r="B172" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C172" t="s">
         <v>0</v>
@@ -3856,7 +3842,7 @@
         <v>2021</v>
       </c>
       <c r="B173" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C173" t="s">
         <v>1</v>
@@ -3870,7 +3856,7 @@
         <v>2021</v>
       </c>
       <c r="B174" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C174" t="s">
         <v>2</v>
@@ -3884,7 +3870,7 @@
         <v>2021</v>
       </c>
       <c r="B175" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C175" t="s">
         <v>3</v>
@@ -3898,7 +3884,7 @@
         <v>2021</v>
       </c>
       <c r="B176" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C176" t="s">
         <v>4</v>
@@ -3912,7 +3898,7 @@
         <v>2021</v>
       </c>
       <c r="B177" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C177" t="s">
         <v>5</v>
@@ -3926,7 +3912,7 @@
         <v>2021</v>
       </c>
       <c r="B178" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C178" t="s">
         <v>6</v>
@@ -3940,7 +3926,7 @@
         <v>2021</v>
       </c>
       <c r="B179" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C179" t="s">
         <v>7</v>
@@ -3954,10 +3940,10 @@
         <v>2021</v>
       </c>
       <c r="B180" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C180" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D180" s="2">
         <v>1</v>
@@ -3968,10 +3954,10 @@
         <v>2021</v>
       </c>
       <c r="B181" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C181" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D181" s="2">
         <v>1</v>
@@ -3982,7 +3968,7 @@
         <v>2021</v>
       </c>
       <c r="B182" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C182" t="s">
         <v>0</v>
@@ -3996,7 +3982,7 @@
         <v>2021</v>
       </c>
       <c r="B183" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C183" t="s">
         <v>1</v>
@@ -4010,7 +3996,7 @@
         <v>2021</v>
       </c>
       <c r="B184" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C184" t="s">
         <v>2</v>
@@ -4024,7 +4010,7 @@
         <v>2021</v>
       </c>
       <c r="B185" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C185" t="s">
         <v>3</v>
@@ -4038,7 +4024,7 @@
         <v>2021</v>
       </c>
       <c r="B186" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C186" t="s">
         <v>4</v>
@@ -4052,7 +4038,7 @@
         <v>2021</v>
       </c>
       <c r="B187" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C187" t="s">
         <v>5</v>
@@ -4066,7 +4052,7 @@
         <v>2021</v>
       </c>
       <c r="B188" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C188" t="s">
         <v>6</v>
@@ -4080,7 +4066,7 @@
         <v>2021</v>
       </c>
       <c r="B189" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C189" t="s">
         <v>7</v>
@@ -4094,10 +4080,10 @@
         <v>2021</v>
       </c>
       <c r="B190" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C190" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D190" s="2">
         <v>1</v>
@@ -4108,10 +4094,10 @@
         <v>2021</v>
       </c>
       <c r="B191" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C191" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D191" s="2">
         <v>0.9</v>
@@ -4122,7 +4108,7 @@
         <v>2021</v>
       </c>
       <c r="B192" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C192" t="s">
         <v>0</v>
@@ -4136,7 +4122,7 @@
         <v>2021</v>
       </c>
       <c r="B193" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C193" t="s">
         <v>1</v>
@@ -4150,7 +4136,7 @@
         <v>2021</v>
       </c>
       <c r="B194" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C194" t="s">
         <v>2</v>
@@ -4164,7 +4150,7 @@
         <v>2021</v>
       </c>
       <c r="B195" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C195" t="s">
         <v>3</v>
@@ -4178,7 +4164,7 @@
         <v>2021</v>
       </c>
       <c r="B196" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C196" t="s">
         <v>4</v>
@@ -4192,7 +4178,7 @@
         <v>2021</v>
       </c>
       <c r="B197" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C197" t="s">
         <v>5</v>
@@ -4206,7 +4192,7 @@
         <v>2021</v>
       </c>
       <c r="B198" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C198" t="s">
         <v>6</v>
@@ -4220,7 +4206,7 @@
         <v>2021</v>
       </c>
       <c r="B199" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C199" t="s">
         <v>7</v>
@@ -4234,10 +4220,10 @@
         <v>2021</v>
       </c>
       <c r="B200" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C200" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D200" s="2">
         <v>1</v>
@@ -4248,10 +4234,10 @@
         <v>2021</v>
       </c>
       <c r="B201" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C201" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D201" s="2">
         <v>0.9</v>
@@ -4262,7 +4248,7 @@
         <v>2021</v>
       </c>
       <c r="B202" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C202" t="s">
         <v>0</v>
@@ -4276,7 +4262,7 @@
         <v>2021</v>
       </c>
       <c r="B203" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C203" t="s">
         <v>1</v>
@@ -4290,7 +4276,7 @@
         <v>2021</v>
       </c>
       <c r="B204" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C204" t="s">
         <v>2</v>
@@ -4304,7 +4290,7 @@
         <v>2021</v>
       </c>
       <c r="B205" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C205" t="s">
         <v>3</v>
@@ -4318,7 +4304,7 @@
         <v>2021</v>
       </c>
       <c r="B206" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C206" t="s">
         <v>4</v>
@@ -4332,7 +4318,7 @@
         <v>2021</v>
       </c>
       <c r="B207" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C207" t="s">
         <v>5</v>
@@ -4346,7 +4332,7 @@
         <v>2021</v>
       </c>
       <c r="B208" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C208" t="s">
         <v>6</v>
@@ -4360,7 +4346,7 @@
         <v>2021</v>
       </c>
       <c r="B209" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C209" t="s">
         <v>7</v>
@@ -4374,10 +4360,10 @@
         <v>2021</v>
       </c>
       <c r="B210" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C210" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D210" s="2">
         <v>1</v>
@@ -4388,10 +4374,10 @@
         <v>2021</v>
       </c>
       <c r="B211" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C211" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D211" s="2">
         <v>0.9</v>
@@ -4402,7 +4388,7 @@
         <v>2021</v>
       </c>
       <c r="B212" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C212" t="s">
         <v>0</v>
@@ -4416,7 +4402,7 @@
         <v>2021</v>
       </c>
       <c r="B213" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C213" t="s">
         <v>1</v>
@@ -4430,7 +4416,7 @@
         <v>2021</v>
       </c>
       <c r="B214" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C214" t="s">
         <v>2</v>
@@ -4444,7 +4430,7 @@
         <v>2021</v>
       </c>
       <c r="B215" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C215" t="s">
         <v>3</v>
@@ -4458,7 +4444,7 @@
         <v>2021</v>
       </c>
       <c r="B216" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C216" t="s">
         <v>4</v>
@@ -4472,7 +4458,7 @@
         <v>2021</v>
       </c>
       <c r="B217" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C217" t="s">
         <v>5</v>
@@ -4486,7 +4472,7 @@
         <v>2021</v>
       </c>
       <c r="B218" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C218" t="s">
         <v>6</v>
@@ -4500,7 +4486,7 @@
         <v>2021</v>
       </c>
       <c r="B219" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C219" t="s">
         <v>7</v>
@@ -4514,10 +4500,10 @@
         <v>2021</v>
       </c>
       <c r="B220" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C220" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D220" s="2">
         <v>1</v>
@@ -4528,10 +4514,10 @@
         <v>2021</v>
       </c>
       <c r="B221" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C221" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D221" s="2">
         <v>1</v>
@@ -4542,7 +4528,7 @@
         <v>2021</v>
       </c>
       <c r="B222" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C222" t="s">
         <v>0</v>
@@ -4556,7 +4542,7 @@
         <v>2021</v>
       </c>
       <c r="B223" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C223" t="s">
         <v>1</v>
@@ -4570,7 +4556,7 @@
         <v>2021</v>
       </c>
       <c r="B224" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C224" t="s">
         <v>2</v>
@@ -4584,7 +4570,7 @@
         <v>2021</v>
       </c>
       <c r="B225" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C225" t="s">
         <v>3</v>
@@ -4598,7 +4584,7 @@
         <v>2021</v>
       </c>
       <c r="B226" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C226" t="s">
         <v>4</v>
@@ -4612,7 +4598,7 @@
         <v>2021</v>
       </c>
       <c r="B227" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C227" t="s">
         <v>5</v>
@@ -4626,7 +4612,7 @@
         <v>2021</v>
       </c>
       <c r="B228" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C228" t="s">
         <v>6</v>
@@ -4640,7 +4626,7 @@
         <v>2021</v>
       </c>
       <c r="B229" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C229" t="s">
         <v>7</v>
@@ -4654,10 +4640,10 @@
         <v>2021</v>
       </c>
       <c r="B230" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C230" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D230" s="2">
         <v>1</v>
@@ -4668,10 +4654,10 @@
         <v>2021</v>
       </c>
       <c r="B231" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C231" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D231" s="2">
         <v>1</v>
@@ -4682,7 +4668,7 @@
         <v>2021</v>
       </c>
       <c r="B232" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C232" t="s">
         <v>0</v>
@@ -4696,7 +4682,7 @@
         <v>2021</v>
       </c>
       <c r="B233" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C233" t="s">
         <v>1</v>
@@ -4710,7 +4696,7 @@
         <v>2021</v>
       </c>
       <c r="B234" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C234" t="s">
         <v>2</v>
@@ -4724,7 +4710,7 @@
         <v>2021</v>
       </c>
       <c r="B235" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C235" t="s">
         <v>3</v>
@@ -4738,7 +4724,7 @@
         <v>2021</v>
       </c>
       <c r="B236" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C236" t="s">
         <v>4</v>
@@ -4752,7 +4738,7 @@
         <v>2021</v>
       </c>
       <c r="B237" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C237" t="s">
         <v>5</v>
@@ -4766,7 +4752,7 @@
         <v>2021</v>
       </c>
       <c r="B238" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C238" t="s">
         <v>6</v>
@@ -4780,7 +4766,7 @@
         <v>2021</v>
       </c>
       <c r="B239" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C239" t="s">
         <v>7</v>
@@ -4794,10 +4780,10 @@
         <v>2021</v>
       </c>
       <c r="B240" t="s">
+        <v>28</v>
+      </c>
+      <c r="C240" t="s">
         <v>30</v>
-      </c>
-      <c r="C240" t="s">
-        <v>33</v>
       </c>
       <c r="D240" s="2">
         <v>1</v>
@@ -4808,10 +4794,10 @@
         <v>2021</v>
       </c>
       <c r="B241" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C241" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D241" s="2">
         <v>1</v>
@@ -4822,7 +4808,7 @@
         <v>2021</v>
       </c>
       <c r="B242" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C242" t="s">
         <v>0</v>
@@ -4836,7 +4822,7 @@
         <v>2021</v>
       </c>
       <c r="B243" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C243" t="s">
         <v>1</v>
@@ -4850,7 +4836,7 @@
         <v>2021</v>
       </c>
       <c r="B244" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C244" t="s">
         <v>2</v>
@@ -4864,7 +4850,7 @@
         <v>2021</v>
       </c>
       <c r="B245" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C245" t="s">
         <v>3</v>
@@ -4878,7 +4864,7 @@
         <v>2021</v>
       </c>
       <c r="B246" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C246" t="s">
         <v>4</v>
@@ -4892,7 +4878,7 @@
         <v>2021</v>
       </c>
       <c r="B247" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C247" t="s">
         <v>5</v>
@@ -4906,7 +4892,7 @@
         <v>2021</v>
       </c>
       <c r="B248" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C248" t="s">
         <v>6</v>
@@ -4920,7 +4906,7 @@
         <v>2021</v>
       </c>
       <c r="B249" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C249" t="s">
         <v>7</v>
@@ -4934,10 +4920,10 @@
         <v>2021</v>
       </c>
       <c r="B250" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C250" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D250" s="2">
         <v>1</v>
@@ -4948,10 +4934,10 @@
         <v>2021</v>
       </c>
       <c r="B251" t="s">
+        <v>29</v>
+      </c>
+      <c r="C251" t="s">
         <v>31</v>
-      </c>
-      <c r="C251" t="s">
-        <v>34</v>
       </c>
       <c r="D251" s="2">
         <v>1</v>
@@ -4978,16 +4964,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="D1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
AS1170 - add a method to determine drag on a rectangle.
</commit_message>
<xml_diff>
--- a/utilityscripts/as1170_2.xlsx
+++ b/utilityscripts/as1170_2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sean Kane\PycharmProjects\utilityscripts\utilityscripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE63E873-0468-40F0-83D2-AF752C874928}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25C4BFEA-897E-43C5-A21F-4897069A4A09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="3" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="3" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="wind_direction_definitions" sheetId="1" r:id="rId1"/>
@@ -22,6 +22,7 @@
     <sheet name="cpi_t5b" sheetId="8" r:id="rId7"/>
     <sheet name="k_a" sheetId="9" r:id="rId8"/>
     <sheet name="cpe_t5_2c" sheetId="10" r:id="rId9"/>
+    <sheet name="app_c_fig_c2" sheetId="11" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="614" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="618" uniqueCount="66">
   <si>
     <t>N</t>
   </si>
@@ -227,6 +228,18 @@
   </si>
   <si>
     <t>distance_edge</t>
+  </si>
+  <si>
+    <t>d_b_ratio</t>
+  </si>
+  <si>
+    <t>theta</t>
+  </si>
+  <si>
+    <t>f_x</t>
+  </si>
+  <si>
+    <t>f_y</t>
   </si>
 </sst>
 </file>
@@ -666,6 +679,293 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57D6BFCE-8807-4FA6-8CAD-90A0E49EBC9F}">
+  <dimension ref="A1:D19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0.1</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>0.33</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>0.4</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>0.62</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>2.8</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>1.6</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>1.7</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>2.5</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>1.5</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>3</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>1.3</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>10</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>0.1</v>
+      </c>
+      <c r="B11">
+        <v>45</v>
+      </c>
+      <c r="C11">
+        <v>1.8</v>
+      </c>
+      <c r="D11">
+        <v>-0.11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>0.33</v>
+      </c>
+      <c r="B12">
+        <v>45</v>
+      </c>
+      <c r="C12">
+        <v>1.7</v>
+      </c>
+      <c r="D12">
+        <v>-0.4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>0.4</v>
+      </c>
+      <c r="B13">
+        <v>45</v>
+      </c>
+      <c r="C13">
+        <v>1.7</v>
+      </c>
+      <c r="D13">
+        <v>-0.52</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>0.62</v>
+      </c>
+      <c r="B14">
+        <v>45</v>
+      </c>
+      <c r="C14">
+        <v>1.7</v>
+      </c>
+      <c r="D14">
+        <v>-0.93</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>1</v>
+      </c>
+      <c r="B15">
+        <v>45</v>
+      </c>
+      <c r="C15">
+        <v>1.5</v>
+      </c>
+      <c r="D15">
+        <v>-1.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>1.6</v>
+      </c>
+      <c r="B16">
+        <v>45</v>
+      </c>
+      <c r="C16">
+        <v>1.5</v>
+      </c>
+      <c r="D16">
+        <v>-2.7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>2.5</v>
+      </c>
+      <c r="B17">
+        <v>45</v>
+      </c>
+      <c r="C17">
+        <v>1.3</v>
+      </c>
+      <c r="D17">
+        <v>-4.2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>3</v>
+      </c>
+      <c r="B18">
+        <v>45</v>
+      </c>
+      <c r="C18">
+        <v>1.2</v>
+      </c>
+      <c r="D18">
+        <v>-5.0999999999999996</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>10</v>
+      </c>
+      <c r="B19">
+        <v>45</v>
+      </c>
+      <c r="C19">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D19">
+        <v>-18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA3FA9CA-B7A2-4CAB-99B0-2332ACD239DB}">
   <dimension ref="A1:C9"/>
@@ -7563,7 +7863,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02C147CC-3A12-402B-BB71-F03DBCCD8C15}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>

</xml_diff>